<commit_message>
update file DB Table
</commit_message>
<xml_diff>
--- a/Documents/DB_Tables_20150110.xlsx
+++ b/Documents/DB_Tables_20150110.xlsx
@@ -138,10 +138,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>NOTICE_MIAGES</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>공지사항 이미지</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -174,10 +170,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>GUIDE_MIAGES</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>GUIDES</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -303,6 +295,14 @@
   </si>
   <si>
     <t>INT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NOTICE_FILES</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GUIDE_FILES</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -667,8 +667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -749,13 +749,13 @@
     </row>
     <row r="8" spans="1:4">
       <c r="B8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C8" t="s">
         <v>26</v>
       </c>
       <c r="D8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -788,7 +788,7 @@
         <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -802,7 +802,7 @@
         <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -810,7 +810,7 @@
         <v>19</v>
       </c>
       <c r="C14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -823,18 +823,18 @@
     </row>
     <row r="16" spans="1:4">
       <c r="B16" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="2" t="s">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="B18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C18" t="s">
         <v>26</v>
@@ -845,7 +845,7 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B19" t="s">
         <v>16</v>
@@ -854,28 +854,28 @@
         <v>26</v>
       </c>
       <c r="D19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="B20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" t="s">
         <v>36</v>
-      </c>
-      <c r="C20" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="B21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B23" t="s">
         <v>16</v>
@@ -920,7 +920,7 @@
         <v>6</v>
       </c>
       <c r="D26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -941,10 +941,10 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="2" t="s">
-        <v>39</v>
+        <v>71</v>
       </c>
       <c r="B30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C30" t="s">
         <v>26</v>
@@ -955,7 +955,7 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B31" t="s">
         <v>16</v>
@@ -964,28 +964,28 @@
         <v>26</v>
       </c>
       <c r="D31" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="B32" t="s">
+        <v>35</v>
+      </c>
+      <c r="C32" t="s">
         <v>36</v>
-      </c>
-      <c r="C32" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="B33" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C33" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B35" t="s">
         <v>16</v>
@@ -999,7 +999,7 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B36" t="s">
         <v>17</v>
@@ -1010,16 +1010,16 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B37" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C37" t="s">
         <v>26</v>
       </c>
       <c r="D37" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1030,12 +1030,12 @@
         <v>6</v>
       </c>
       <c r="D38" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="B39" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C39" t="s">
         <v>26</v>
@@ -1043,7 +1043,7 @@
     </row>
     <row r="40" spans="1:4">
       <c r="B40" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C40" t="s">
         <v>26</v>
@@ -1051,7 +1051,7 @@
     </row>
     <row r="41" spans="1:4">
       <c r="B41" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C41" t="s">
         <v>6</v>
@@ -1059,7 +1059,7 @@
     </row>
     <row r="42" spans="1:4">
       <c r="B42" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C42" t="s">
         <v>6</v>
@@ -1067,18 +1067,18 @@
     </row>
     <row r="43" spans="1:4">
       <c r="B43" t="s">
+        <v>51</v>
+      </c>
+      <c r="C43" t="s">
         <v>53</v>
-      </c>
-      <c r="C43" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="B44" t="s">
+        <v>52</v>
+      </c>
+      <c r="C44" t="s">
         <v>54</v>
-      </c>
-      <c r="C44" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1099,10 +1099,10 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B48" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C48" t="s">
         <v>26</v>
@@ -1113,7 +1113,7 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B49" t="s">
         <v>16</v>
@@ -1122,31 +1122,31 @@
         <v>26</v>
       </c>
       <c r="D49" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B50" t="s">
+        <v>35</v>
+      </c>
+      <c r="C50" t="s">
         <v>36</v>
-      </c>
-      <c r="C50" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="B51" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C51" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B53" t="s">
         <v>16</v>
@@ -1160,7 +1160,7 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B54" t="s">
         <v>17</v>
@@ -1177,23 +1177,23 @@
         <v>6</v>
       </c>
       <c r="D55" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="B56" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C56" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="B57" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C57" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -1214,35 +1214,35 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B61" t="s">
+        <v>35</v>
+      </c>
+      <c r="C61" t="s">
         <v>36</v>
-      </c>
-      <c r="C61" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C62" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="B63" t="s">
+        <v>60</v>
+      </c>
+      <c r="C63" t="s">
+        <v>36</v>
+      </c>
+      <c r="D63" t="s">
         <v>62</v>
-      </c>
-      <c r="C63" t="s">
-        <v>37</v>
-      </c>
-      <c r="D63" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="64" spans="1:4">

</xml_diff>